<commit_message>
My Worse commit yet. Nothing works but I get off work in 20 mins. Will have to fix monday.
worked on specsfile parser that takes an EML and parsers it to my Global variables

from that we use the globals we got from the EML to put into an EXcel sheet

Ip address doesnt work, Theres no correction function to ask if the EML parse was right, and Optional Excel Variables arent handled yet.

Added SHA256fromString I have no clue if it works yet, Used for other modules to get there formatted file SHA hash
</commit_message>
<xml_diff>
--- a/Program/Files/WalkerTA-MISP-Template.xlsx
+++ b/Program/Files/WalkerTA-MISP-Template.xlsx
@@ -1028,7 +1028,7 @@
       <c r="C22" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D22" s="3" t="n"/>
+      <c r="D22" s="3" t="inlineStr"/>
       <c r="E22" s="11" t="inlineStr">
         <is>
           <t>Artifacts dropped (file)</t>
@@ -1049,7 +1049,7 @@
       <c r="C23" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D23" s="3" t="n"/>
+      <c r="D23" s="3" t="inlineStr"/>
       <c r="E23" s="11" t="inlineStr">
         <is>
           <t>Artifacts dropped (file)</t>
@@ -1070,7 +1070,7 @@
       <c r="C24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D24" s="3" t="n"/>
+      <c r="D24" s="3" t="inlineStr"/>
       <c r="E24" s="11" t="inlineStr">
         <is>
           <t>Artifacts dropped (file)</t>
@@ -1091,7 +1091,7 @@
       <c r="C25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D25" s="3" t="n"/>
+      <c r="D25" s="3" t="inlineStr"/>
       <c r="E25" s="11" t="inlineStr">
         <is>
           <t>Artifacts dropped (file)</t>
@@ -1112,7 +1112,7 @@
       <c r="C26" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D26" s="3" t="n"/>
+      <c r="D26" s="3" t="inlineStr"/>
       <c r="E26" s="11" t="inlineStr">
         <is>
           <t>Artifacts dropped (file)</t>
@@ -1154,7 +1154,7 @@
       <c r="C28" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D28" s="3" t="n"/>
+      <c r="D28" s="3" t="inlineStr"/>
       <c r="E28" s="11" t="inlineStr">
         <is>
           <t>Credential POST</t>
@@ -1175,7 +1175,7 @@
       <c r="C29" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D29" s="3" t="n"/>
+      <c r="D29" s="3" t="inlineStr"/>
       <c r="E29" s="11" t="inlineStr">
         <is>
           <t>Redirect URL</t>
@@ -1196,7 +1196,7 @@
       <c r="C30" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D30" s="3" t="n"/>
+      <c r="D30" s="3" t="inlineStr"/>
       <c r="E30" s="11" t="inlineStr">
         <is>
           <t>Redirect URL</t>
@@ -1217,7 +1217,7 @@
       <c r="C31" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D31" s="3" t="n"/>
+      <c r="D31" s="3" t="inlineStr"/>
       <c r="E31" s="11" t="inlineStr">
         <is>
           <t>Redirect URL</t>
@@ -1238,7 +1238,7 @@
       <c r="C32" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D32" s="3" t="n"/>
+      <c r="D32" s="3" t="inlineStr"/>
       <c r="E32" s="11" t="inlineStr">
         <is>
           <t>Redirect URL</t>
@@ -1259,7 +1259,7 @@
       <c r="C33" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D33" s="3" t="n"/>
+      <c r="D33" s="3" t="inlineStr"/>
       <c r="E33" s="11" t="inlineStr">
         <is>
           <t>Redirect URL</t>
@@ -1280,7 +1280,7 @@
       <c r="C34" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D34" s="3" t="n"/>
+      <c r="D34" s="3" t="inlineStr"/>
       <c r="E34" s="11" t="inlineStr">
         <is>
           <t>Research links</t>
@@ -1301,7 +1301,7 @@
       <c r="C35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D35" s="3" t="n"/>
+      <c r="D35" s="3" t="inlineStr"/>
       <c r="E35" s="11" t="inlineStr">
         <is>
           <t>Research links</t>
@@ -1322,7 +1322,7 @@
       <c r="C36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D36" s="3" t="n"/>
+      <c r="D36" s="3" t="inlineStr"/>
       <c r="E36" s="11" t="inlineStr">
         <is>
           <t>Research links</t>
@@ -1343,7 +1343,7 @@
       <c r="C37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D37" s="3" t="n"/>
+      <c r="D37" s="3" t="inlineStr"/>
       <c r="E37" s="11" t="inlineStr">
         <is>
           <t>Research links</t>
@@ -1364,7 +1364,7 @@
       <c r="C38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="D38" s="3" t="n"/>
+      <c r="D38" s="3" t="inlineStr"/>
       <c r="E38" s="11" t="inlineStr">
         <is>
           <t>Research links</t>

</xml_diff>